<commit_message>
Updated w/ Forecasts for 1st March
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53CE64A-250D-E244-BA03-A65803BB5E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D95D23-9E1B-714B-8A16-A884A5859CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
+    <workbookView xWindow="4740" yWindow="460" windowWidth="23260" windowHeight="16160" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,7 @@
   <dimension ref="A1:AB34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,16 +1169,54 @@
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
+      <c r="B18" s="18">
+        <v>10.21856</v>
+      </c>
+      <c r="C18" s="18">
+        <v>4.9150489999999998E-2</v>
+      </c>
+      <c r="D18">
+        <v>10.2479126841792</v>
+      </c>
+      <c r="E18">
+        <v>3.00047010642495E-2</v>
+      </c>
+      <c r="F18" s="18">
+        <v>10.20628</v>
+      </c>
+      <c r="G18" s="18">
+        <v>6.3572959999999998E-2</v>
+      </c>
+      <c r="H18" s="20">
+        <v>10.224</v>
+      </c>
+      <c r="I18" s="20">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="J18" s="18">
+        <v>10.247249999999999</v>
+      </c>
+      <c r="K18" s="18">
+        <v>4.6216849999999997E-2</v>
+      </c>
+      <c r="L18" s="20">
+        <v>10.20459</v>
+      </c>
+      <c r="M18" s="20">
+        <v>4.8135659999999997E-2</v>
+      </c>
+      <c r="N18" s="18">
+        <v>10.185255</v>
+      </c>
+      <c r="O18" s="18">
+        <v>5.9166290000000003E-2</v>
+      </c>
+      <c r="P18" s="20">
+        <v>10.21345</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>4.888E-2</v>
+      </c>
       <c r="T18" s="6" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Second to last Round
</commit_message>
<xml_diff>
--- a/Scoring Forecasting Competition.xlsx
+++ b/Scoring Forecasting Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nz3618/Desktop/Forecasting Competition/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9968E329-B67D-B34D-AC63-D99FCD32C97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F895E1FE-D213-8842-9FF6-3A70669063CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="460" windowWidth="23260" windowHeight="16160" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
+    <workbookView xWindow="3660" yWindow="460" windowWidth="24340" windowHeight="16160" xr2:uid="{198224F8-EE29-E944-BE8A-D9E813220B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967CD6C7-451E-0748-9748-9A42CF32D73A}">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="96" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,35 +664,35 @@
       </c>
       <c r="B2" s="20">
         <f>SUMIF($J25:$J34,"&lt;&gt;#NUM!")</f>
-        <v>9.7433124860919769</v>
+        <v>11.316063526115544</v>
       </c>
       <c r="C2" s="20">
         <f>SUMIF($B25:$B34,"&lt;&gt;#NUM!")</f>
-        <v>8.0492642969715114</v>
+        <v>9.9358931414994238</v>
       </c>
       <c r="D2" s="20">
         <f>SUMIF($H25:$H34,"&lt;&gt;#NUM!")</f>
-        <v>7.4446942138117951</v>
+        <v>9.6442705105794921</v>
       </c>
       <c r="E2" s="20">
         <f>SUMIF($L25:$L34,"&lt;&gt;#NUM!")</f>
-        <v>4.2833513953049041</v>
+        <v>6.3582330005706735</v>
       </c>
       <c r="F2" s="20">
         <f>SUMIF($P25:$P34,"&lt;&gt;#NUM!")</f>
-        <v>-0.33940517476017618</v>
+        <v>1.7565172080304863</v>
       </c>
       <c r="G2" s="20">
         <f>SUMIF($F25:$F34,"&lt;&gt;#NUM!")</f>
-        <v>-1.2937259148958735</v>
+        <v>3.0064647122320709E-2</v>
       </c>
       <c r="H2" s="20">
         <f>SUMIF($N25:$N34,"&lt;&gt;#NUM!")</f>
-        <v>-1.7874990494700194</v>
+        <v>-0.33606720988131711</v>
       </c>
       <c r="I2" s="20">
         <f>SUMIF($D25:$D34,"&lt;&gt;#NUM!")</f>
-        <v>-3.2067198342261172</v>
+        <v>-1.2625952403869991</v>
       </c>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
@@ -1228,34 +1228,113 @@
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
+      <c r="B19" s="18">
+        <v>10.30555</v>
+      </c>
+      <c r="C19" s="18">
+        <v>5.9181879999999999E-2</v>
+      </c>
+      <c r="D19">
+        <v>10.284708709657</v>
+      </c>
+      <c r="E19">
+        <v>4.1530461453203903E-2</v>
+      </c>
+      <c r="F19" s="18">
+        <v>10.25404</v>
+      </c>
+      <c r="G19" s="18">
+        <v>5.8132049999999998E-2</v>
+      </c>
+      <c r="H19" s="20">
+        <v>10.297283999999999</v>
+      </c>
+      <c r="I19" s="20">
+        <v>3.8285E-2</v>
+      </c>
+      <c r="J19" s="24">
+        <v>10.269780000000001</v>
+      </c>
+      <c r="K19" s="24">
+        <v>3.9542420000000002E-2</v>
+      </c>
+      <c r="L19" s="20">
+        <v>10.309089999999999</v>
+      </c>
+      <c r="M19" s="20">
+        <v>4.9312740000000001E-2</v>
+      </c>
+      <c r="N19" s="18">
+        <v>10.279210000000001</v>
+      </c>
+      <c r="O19" s="18">
+        <v>8.4085999999999994E-2</v>
+      </c>
+      <c r="P19" s="20">
+        <v>10.314109999999999</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>4.8910000000000002E-2</v>
+      </c>
       <c r="T19" s="6" t="s">
         <v>28</v>
+      </c>
+      <c r="U19">
+        <v>30267.895833333299</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="B20" s="18">
+        <v>10.34582</v>
+      </c>
+      <c r="C20" s="18">
+        <v>4.1997199999999998E-2</v>
+      </c>
+      <c r="D20">
+        <v>10.3391328841569</v>
+      </c>
+      <c r="E20">
+        <v>3.1128680256294401E-2</v>
+      </c>
+      <c r="F20" s="18">
+        <v>10.25417</v>
+      </c>
+      <c r="G20" s="18">
+        <v>5.8094279999999998E-2</v>
+      </c>
+      <c r="H20" s="20">
+        <v>10.193564</v>
+      </c>
+      <c r="I20" s="20">
+        <v>4.3531986729803698E-2</v>
+      </c>
+      <c r="J20" s="24">
+        <v>10.20565</v>
+      </c>
+      <c r="K20" s="24">
+        <v>3.6771190000000002E-2</v>
+      </c>
+      <c r="L20" s="25">
+        <v>10.21313</v>
+      </c>
+      <c r="M20" s="25">
+        <v>4.9336039999999998E-2</v>
+      </c>
+      <c r="N20" s="18">
+        <v>10.281853</v>
+      </c>
+      <c r="O20" s="18">
+        <v>8.4030999999999995E-2</v>
+      </c>
+      <c r="P20" s="20">
+        <v>10.254289999999999</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>4.8379999999999999E-2</v>
+      </c>
       <c r="T20" s="6" t="s">
         <v>29</v>
       </c>
@@ -1574,41 +1653,41 @@
       <c r="A31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="18" t="e">
+      <c r="B31" s="18">
         <f t="shared" si="1"/>
-        <v>#NUM!</v>
+        <v>1.8866288445279131</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="20" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="F31" s="18" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="D31" s="20">
+        <f t="shared" si="0"/>
+        <v>1.9441245938391181</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="0"/>
+        <v>1.3237905620181942</v>
       </c>
       <c r="G31" s="18"/>
-      <c r="H31" s="20" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J31" s="18" t="e">
+      <c r="H31" s="20">
+        <f t="shared" si="0"/>
+        <v>2.1995762967676971</v>
+      </c>
+      <c r="J31" s="18">
         <f t="shared" si="2"/>
-        <v>#NUM!</v>
+        <v>1.5727510400235662</v>
       </c>
       <c r="K31" s="18"/>
-      <c r="L31" s="20" t="e">
+      <c r="L31" s="20">
         <f>LN( _xlfn.NORM.DIST( LN($U19), L19, M19, 0 ) )</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N31" s="18" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>2.0748816052657695</v>
+      </c>
+      <c r="N31" s="18">
+        <f t="shared" si="0"/>
+        <v>1.4514318395887023</v>
       </c>
       <c r="O31" s="18"/>
-      <c r="P31" s="20" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
+      <c r="P31" s="20">
+        <f t="shared" si="0"/>
+        <v>2.0959223827906626</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="20" x14ac:dyDescent="0.25">

</xml_diff>